<commit_message>
Modeli definitivo, modificacion de documento
</commit_message>
<xml_diff>
--- a/Data-Burgoin.xlsx
+++ b/Data-Burgoin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="11715" windowHeight="7620"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="11715" windowHeight="7620" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="28-04-13" sheetId="1" r:id="rId1"/>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:M23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E16" sqref="E6:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3403,12 +3403,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="P3:AE3"/>
     <mergeCell ref="AF3:AF5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -3421,6 +3415,12 @@
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="T4:U4"/>
     <mergeCell ref="V4:W4"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="P3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3430,8 +3430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3490,17 +3490,26 @@
         <f>SQRT(SUMSQ(Q2:Q42)/COUNTA(Q2:Q42))</f>
         <v>12.022876428138883</v>
       </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
       <c r="S1" s="79">
         <f>SQRT(SUMSQ(S2:S42)/COUNTA(S2:S42))</f>
         <v>10.128265491669591</v>
       </c>
+      <c r="T1">
+        <v>2</v>
+      </c>
       <c r="U1" s="79">
         <f>SQRT(SUMSQ(U2:U42)/COUNTA(U2:U42))</f>
         <v>7.229450832493427</v>
       </c>
+      <c r="V1">
+        <v>5</v>
+      </c>
       <c r="W1" s="79">
         <f>SQRT(SUMSQ(W2:W42)/COUNTA(W2:W42))</f>
-        <v>11.764048385785532</v>
+        <v>11.547039077555084</v>
       </c>
       <c r="X1" s="75"/>
       <c r="Y1" s="79">
@@ -3576,28 +3585,28 @@
         <v>-14.383319999999998</v>
       </c>
       <c r="R2">
-        <f t="shared" ref="R2:R42" si="6" xml:space="preserve"> -0.0000003143*(C2)^3 + 0.0005606*(C2)^2 - 0.01602*(C2) + 75.46</f>
+        <f t="shared" ref="R2:R44" si="6" xml:space="preserve"> -0.0000003143*(C2)^3 + 0.0005606*(C2)^2 - 0.01602*(C2) + 75.46</f>
         <v>75.444050886399992</v>
       </c>
       <c r="S2" s="80">
-        <f t="shared" ref="S2:S42" si="7">K2-R2</f>
+        <f t="shared" ref="S2:S44" si="7">K2-R2</f>
         <v>-12.444050886399992</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T42" si="8" xml:space="preserve"> 76.44 - (0.08533*C2) - (0.003054*E2) + (0.004229*(C2)^2) - (0.002185*C2*E2) + (0.0002715*(E2)^2) - (0.000003174*((C2)^2)*E2) + (0.000001423*C2*(E2)^2) - (0.0000001513*(E2)^3)</f>
+        <f t="shared" ref="T2:T44" si="8" xml:space="preserve"> 76.44 - (0.08533*C2) - (0.003054*E2) + (0.004229*(C2)^2) - (0.002185*C2*E2) + (0.0002715*(E2)^2) - (0.000003174*((C2)^2)*E2) + (0.000001423*C2*(E2)^2) - (0.0000001513*(E2)^3)</f>
         <v>73.77286725999997</v>
       </c>
       <c r="U2" s="80">
-        <f t="shared" ref="U2:U42" si="9">K2-T2</f>
+        <f t="shared" ref="U2:U44" si="9">K2-T2</f>
         <v>-10.77286725999997</v>
       </c>
       <c r="V2">
-        <f>426.44 + 0.0035805*C2 + 0.020846*E2 - 56.528*A2 + 2.1107*G2</f>
-        <v>75.613694000000038</v>
+        <f>425 + 0.045635*C2 + 0.01423*E2 - 56.6*A2 + 2.127*G2</f>
+        <v>74.61948000000001</v>
       </c>
       <c r="W2" s="80">
         <f>K2-V2</f>
-        <v>-12.613694000000038</v>
+        <v>-11.61948000000001</v>
       </c>
       <c r="X2" s="15">
         <f xml:space="preserve"> 95.72 - 1.33*C2 - 0.07005*E2 + 0.04464*C2^2 - 0.01072*C2*E2 + 0.001403*E2^2 - 0.0004819*C2^3 + 0.0002204*C2^2*E2 - 0.00002532*C2*E2^2 + 0.0000009191*C2^4 - 0.0000004632642*C2^3*E2 + 0.00000005263*C2^2*E2^2</f>
@@ -3699,12 +3708,12 @@
         <v>4.802013720000005</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V42" si="10">426.44 + 0.0035805*C3 + 0.020846*E3 - 56.528*A3 + 2.1107*G3</f>
-        <v>76.328586500000057</v>
+        <f t="shared" ref="V3:V44" si="10">425 + 0.045635*C3 + 0.01423*E3 - 56.6*A3 + 2.127*G3</f>
+        <v>76.187254999999993</v>
       </c>
       <c r="W3" s="80">
-        <f t="shared" ref="W3:W42" si="11">K3-V3</f>
-        <v>1.671413499999943</v>
+        <f t="shared" ref="W3:W44" si="11">K3-V3</f>
+        <v>1.8127450000000067</v>
       </c>
       <c r="X3" s="15">
         <f t="shared" ref="X3:X42" si="12" xml:space="preserve"> 95.72 - 1.33*C3 - 0.07005*E3 + 0.04464*C3^2 - 0.01072*C3*E3 + 0.001403*E3^2 - 0.0004819*C3^3 + 0.0002204*C3^2*E3 - 0.00002532*C3*E3^2 + 0.0000009191*C3^4 - 0.0000004632642*C3^3*E3 + 0.00000005263*C3^2*E3^2</f>
@@ -3807,11 +3816,11 @@
       </c>
       <c r="V4">
         <f t="shared" si="10"/>
-        <v>75.836476000000033</v>
+        <v>74.944320000000005</v>
       </c>
       <c r="W4" s="80">
         <f t="shared" si="11"/>
-        <v>-2.8364760000000331</v>
+        <v>-1.9443200000000047</v>
       </c>
       <c r="X4" s="15">
         <f t="shared" si="12"/>
@@ -3917,11 +3926,11 @@
       </c>
       <c r="V5">
         <f t="shared" si="10"/>
-        <v>75.829315000000037</v>
+        <v>74.853049999999996</v>
       </c>
       <c r="W5" s="80">
         <f t="shared" si="11"/>
-        <v>-12.829315000000037</v>
+        <v>-11.853049999999996</v>
       </c>
       <c r="X5" s="15">
         <f t="shared" si="12"/>
@@ -4024,11 +4033,11 @@
       </c>
       <c r="V6">
         <f t="shared" si="10"/>
-        <v>75.398073000000039</v>
+        <v>74.385909999999967</v>
       </c>
       <c r="W6" s="80">
         <f t="shared" si="11"/>
-        <v>-12.398073000000039</v>
+        <v>-11.385909999999967</v>
       </c>
       <c r="X6" s="15">
         <f t="shared" si="12"/>
@@ -4131,11 +4140,11 @@
       </c>
       <c r="V7">
         <f t="shared" si="10"/>
-        <v>75.380170500000048</v>
+        <v>74.157734999999946</v>
       </c>
       <c r="W7" s="80">
         <f t="shared" si="11"/>
-        <v>-12.380170500000048</v>
+        <v>-11.157734999999946</v>
       </c>
       <c r="X7" s="15">
         <f t="shared" si="12"/>
@@ -4238,11 +4247,11 @@
       </c>
       <c r="V8">
         <f t="shared" si="10"/>
-        <v>75.20393500000003</v>
+        <v>74.426150000000007</v>
       </c>
       <c r="W8" s="80">
         <f t="shared" si="11"/>
-        <v>-12.20393500000003</v>
+        <v>-11.426150000000007</v>
       </c>
       <c r="X8" s="15">
         <f t="shared" si="12"/>
@@ -4345,11 +4354,11 @@
       </c>
       <c r="V9">
         <f t="shared" si="10"/>
-        <v>74.966831000000042</v>
+        <v>73.918769999999938</v>
       </c>
       <c r="W9" s="80">
         <f t="shared" si="11"/>
-        <v>-11.966831000000042</v>
+        <v>-10.918769999999938</v>
       </c>
       <c r="X9" s="15">
         <f t="shared" si="12"/>
@@ -4455,11 +4464,11 @@
       </c>
       <c r="V10">
         <f t="shared" si="10"/>
-        <v>74.744049000000047</v>
+        <v>73.59393</v>
       </c>
       <c r="W10" s="80">
         <f t="shared" si="11"/>
-        <v>-11.744049000000047</v>
+        <v>-10.59393</v>
       </c>
       <c r="X10" s="15">
         <f t="shared" si="12"/>
@@ -4562,11 +4571,11 @@
       </c>
       <c r="V11">
         <f t="shared" si="10"/>
-        <v>74.722566</v>
+        <v>73.320119999999974</v>
       </c>
       <c r="W11" s="80">
         <f t="shared" si="11"/>
-        <v>-11.722566</v>
+        <v>-10.320119999999974</v>
       </c>
       <c r="X11" s="15">
         <f t="shared" si="12"/>
@@ -4669,11 +4678,11 @@
       </c>
       <c r="V12">
         <f t="shared" si="10"/>
-        <v>73.952351000000036</v>
+        <v>72.79736999999993</v>
       </c>
       <c r="W12" s="80">
         <f t="shared" si="11"/>
-        <v>-1.9523510000000357</v>
+        <v>-0.79736999999992975</v>
       </c>
       <c r="X12" s="15">
         <f t="shared" si="12"/>
@@ -4776,11 +4785,11 @@
       </c>
       <c r="V13">
         <f t="shared" si="10"/>
-        <v>73.941609500000041</v>
+        <v>72.660464999999974</v>
       </c>
       <c r="W13" s="80">
         <f t="shared" si="11"/>
-        <v>4.0583904999999589</v>
+        <v>5.3395350000000263</v>
       </c>
       <c r="X13" s="15">
         <f t="shared" si="12"/>
@@ -4883,11 +4892,11 @@
       </c>
       <c r="V14">
         <f t="shared" si="10"/>
-        <v>73.948770500000037</v>
+        <v>72.751734999999925</v>
       </c>
       <c r="W14" s="80">
         <f t="shared" si="11"/>
-        <v>4.0512294999999625</v>
+        <v>5.2482650000000746</v>
       </c>
       <c r="X14" s="15">
         <f t="shared" si="12"/>
@@ -4990,11 +4999,11 @@
       </c>
       <c r="V15">
         <f t="shared" si="10"/>
-        <v>73.938029000000043</v>
+        <v>72.614829999999969</v>
       </c>
       <c r="W15" s="80">
         <f t="shared" si="11"/>
-        <v>4.0619709999999571</v>
+        <v>5.3851700000000307</v>
       </c>
       <c r="X15" s="15">
         <f t="shared" si="12"/>
@@ -5097,11 +5106,11 @@
       </c>
       <c r="V16">
         <f t="shared" si="10"/>
-        <v>73.941609500000041</v>
+        <v>72.660464999999974</v>
       </c>
       <c r="W16" s="80">
         <f t="shared" si="11"/>
-        <v>4.0583904999999589</v>
+        <v>5.3395350000000263</v>
       </c>
       <c r="X16" s="15">
         <f t="shared" si="12"/>
@@ -5204,11 +5213,11 @@
       </c>
       <c r="V17">
         <f t="shared" si="10"/>
-        <v>73.941609500000041</v>
+        <v>72.660464999999974</v>
       </c>
       <c r="W17" s="80">
         <f t="shared" si="11"/>
-        <v>4.0583904999999589</v>
+        <v>5.3395350000000263</v>
       </c>
       <c r="X17" s="15">
         <f t="shared" si="12"/>
@@ -5311,11 +5320,11 @@
       </c>
       <c r="V18">
         <f t="shared" si="10"/>
-        <v>73.945190000000039</v>
+        <v>72.706099999999921</v>
       </c>
       <c r="W18" s="80">
         <f t="shared" si="11"/>
-        <v>4.0548099999999607</v>
+        <v>5.2939000000000789</v>
       </c>
       <c r="X18" s="15">
         <f t="shared" si="12"/>
@@ -5418,11 +5427,11 @@
       </c>
       <c r="V19">
         <f t="shared" si="10"/>
-        <v>73.96309250000003</v>
+        <v>72.934274999999943</v>
       </c>
       <c r="W19" s="80">
         <f t="shared" si="11"/>
-        <v>4.0369074999999697</v>
+        <v>5.0657250000000573</v>
       </c>
       <c r="X19" s="15">
         <f t="shared" si="12"/>
@@ -5525,11 +5534,11 @@
       </c>
       <c r="V20">
         <f t="shared" si="10"/>
-        <v>73.521109000000038</v>
+        <v>72.330229999999958</v>
       </c>
       <c r="W20" s="80">
         <f t="shared" si="11"/>
-        <v>4.4788909999999618</v>
+        <v>5.6697700000000424</v>
       </c>
       <c r="X20" s="15">
         <f t="shared" si="12"/>
@@ -5632,11 +5641,11 @@
       </c>
       <c r="V21">
         <f t="shared" si="10"/>
-        <v>73.524689500000036</v>
+        <v>72.375864999999962</v>
       </c>
       <c r="W21" s="80">
         <f t="shared" si="11"/>
-        <v>4.4753104999999636</v>
+        <v>5.6241350000000381</v>
       </c>
       <c r="X21" s="15">
         <f t="shared" si="12"/>
@@ -5739,11 +5748,11 @@
       </c>
       <c r="V22">
         <f t="shared" si="10"/>
-        <v>73.29116599999999</v>
+        <v>71.914119999999954</v>
       </c>
       <c r="W22" s="80">
         <f t="shared" si="11"/>
-        <v>4.7088340000000102</v>
+        <v>6.0858800000000457</v>
       </c>
       <c r="X22" s="15">
         <f t="shared" si="12"/>
@@ -5846,11 +5855,11 @@
       </c>
       <c r="V23">
         <f t="shared" si="10"/>
-        <v>73.284004999999993</v>
+        <v>71.822849999999946</v>
       </c>
       <c r="W23" s="80">
         <f t="shared" si="11"/>
-        <v>4.7159950000000066</v>
+        <v>6.1771500000000543</v>
       </c>
       <c r="X23" s="15">
         <f t="shared" si="12"/>
@@ -5953,11 +5962,11 @@
       </c>
       <c r="V24">
         <f t="shared" si="10"/>
-        <v>272.27485000000007</v>
+        <v>274.24350000000004</v>
       </c>
       <c r="W24" s="80">
         <f t="shared" si="11"/>
-        <v>-20.274850000000072</v>
+        <v>-22.24350000000004</v>
       </c>
       <c r="X24" s="15">
         <f t="shared" si="12"/>
@@ -6063,11 +6072,11 @@
       </c>
       <c r="V25">
         <f t="shared" si="10"/>
-        <v>154.29198500000004</v>
+        <v>153.53795000000002</v>
       </c>
       <c r="W25" s="80">
         <f t="shared" si="11"/>
-        <v>49.708014999999961</v>
+        <v>50.462049999999977</v>
       </c>
       <c r="X25" s="15">
         <f t="shared" si="12"/>
@@ -6170,11 +6179,11 @@
       </c>
       <c r="V26">
         <f t="shared" si="10"/>
-        <v>121.25012500000001</v>
+        <v>118.27674999999995</v>
       </c>
       <c r="W26" s="80">
         <f t="shared" si="11"/>
-        <v>4.7498749999999887</v>
+        <v>7.7232500000000499</v>
       </c>
       <c r="X26" s="15">
         <f t="shared" si="12"/>
@@ -6277,11 +6286,11 @@
       </c>
       <c r="V27">
         <f t="shared" si="10"/>
-        <v>98.445354999999978</v>
+        <v>95.547850000000039</v>
       </c>
       <c r="W27" s="80">
         <f t="shared" si="11"/>
-        <v>1.554645000000022</v>
+        <v>4.4521499999999605</v>
       </c>
       <c r="X27" s="15">
         <f t="shared" si="12"/>
@@ -6384,11 +6393,11 @@
       </c>
       <c r="V28">
         <f t="shared" si="10"/>
-        <v>87.807525000000027</v>
+        <v>85.694749999999999</v>
       </c>
       <c r="W28" s="80">
         <f t="shared" si="11"/>
-        <v>-3.8075250000000267</v>
+        <v>-1.6947499999999991</v>
       </c>
       <c r="X28" s="15">
         <f t="shared" si="12"/>
@@ -6491,11 +6500,11 @@
       </c>
       <c r="V29">
         <f t="shared" si="10"/>
-        <v>98.10450000000003</v>
+        <v>108.78400000000002</v>
       </c>
       <c r="W29" s="80">
         <f t="shared" si="11"/>
-        <v>11.89549999999997</v>
+        <v>1.2159999999999798</v>
       </c>
       <c r="X29" s="15">
         <f t="shared" si="12"/>
@@ -6599,11 +6608,11 @@
       </c>
       <c r="V30">
         <f t="shared" si="10"/>
-        <v>93.405386000000021</v>
+        <v>99.184020000000004</v>
       </c>
       <c r="W30" s="80">
         <f t="shared" si="11"/>
-        <v>-9.4053860000000213</v>
+        <v>-15.184020000000004</v>
       </c>
       <c r="X30" s="15">
         <f t="shared" si="12"/>
@@ -6709,11 +6718,11 @@
       </c>
       <c r="V31">
         <f t="shared" si="10"/>
-        <v>84.932509000000039</v>
+        <v>86.748830000000027</v>
       </c>
       <c r="W31" s="80">
         <f t="shared" si="11"/>
-        <v>-0.93250900000003867</v>
+        <v>-2.7488300000000265</v>
       </c>
       <c r="X31" s="15">
         <f t="shared" si="12"/>
@@ -6817,11 +6826,11 @@
       </c>
       <c r="V32">
         <f t="shared" si="10"/>
-        <v>84.354466500000058</v>
+        <v>84.410654999999991</v>
       </c>
       <c r="W32" s="80">
         <f t="shared" si="11"/>
-        <v>-4.3544665000000577</v>
+        <v>-4.4106549999999913</v>
       </c>
       <c r="X32" s="15">
         <f t="shared" si="12"/>
@@ -6925,11 +6934,11 @@
       </c>
       <c r="V33">
         <f t="shared" si="10"/>
-        <v>84.085138000000029</v>
+        <v>83.492559999999997</v>
       </c>
       <c r="W33" s="80">
         <f t="shared" si="11"/>
-        <v>-4.085138000000029</v>
+        <v>-3.4925599999999974</v>
       </c>
       <c r="X33" s="15">
         <f t="shared" si="12"/>
@@ -7033,11 +7042,11 @@
       </c>
       <c r="V34">
         <f t="shared" si="10"/>
-        <v>84.06365500000004</v>
+        <v>83.218750000000028</v>
       </c>
       <c r="W34" s="80">
         <f t="shared" si="11"/>
-        <v>-4.0636550000000398</v>
+        <v>-3.2187500000000284</v>
       </c>
       <c r="X34" s="15">
         <f t="shared" si="12"/>
@@ -7141,11 +7150,11 @@
       </c>
       <c r="V35">
         <f t="shared" si="10"/>
-        <v>84.060074500000042</v>
+        <v>83.173115000000024</v>
       </c>
       <c r="W35" s="80">
         <f t="shared" si="11"/>
-        <v>-4.0600745000000416</v>
+        <v>-3.1731150000000241</v>
       </c>
       <c r="X35" s="15">
         <f t="shared" si="12"/>
@@ -7249,11 +7258,11 @@
       </c>
       <c r="V36">
         <f t="shared" si="10"/>
-        <v>83.805068000000063</v>
+        <v>82.437559999999991</v>
       </c>
       <c r="W36" s="80">
         <f t="shared" si="11"/>
-        <v>-3.8050680000000625</v>
+        <v>-2.4375599999999906</v>
       </c>
       <c r="X36" s="15">
         <f t="shared" si="12"/>
@@ -7359,11 +7368,11 @@
       </c>
       <c r="V37">
         <f t="shared" si="10"/>
-        <v>83.589447000000007</v>
+        <v>82.203990000000005</v>
       </c>
       <c r="W37" s="80">
         <f t="shared" si="11"/>
-        <v>-9.5894470000000069</v>
+        <v>-8.2039900000000046</v>
       </c>
       <c r="X37" s="15">
         <f t="shared" si="12"/>
@@ -7466,11 +7475,11 @@
       </c>
       <c r="V38">
         <f t="shared" si="10"/>
-        <v>83.373826000000008</v>
+        <v>81.970419999999962</v>
       </c>
       <c r="W38" s="80">
         <f t="shared" si="11"/>
-        <v>-9.3738260000000082</v>
+        <v>-7.9704199999999616</v>
       </c>
       <c r="X38" s="15">
         <f t="shared" si="12"/>
@@ -7573,11 +7582,11 @@
       </c>
       <c r="V39">
         <f t="shared" si="10"/>
-        <v>79.858542499999999</v>
+        <v>80.922474999999991</v>
       </c>
       <c r="W39" s="80">
         <f t="shared" si="11"/>
-        <v>-8.8585424999999987</v>
+        <v>-9.9224749999999915</v>
       </c>
       <c r="X39" s="15">
         <f t="shared" si="12"/>
@@ -7680,11 +7689,11 @@
       </c>
       <c r="V40">
         <f t="shared" si="10"/>
-        <v>83.48671250000001</v>
+        <v>89.445874999999972</v>
       </c>
       <c r="W40" s="80">
         <f t="shared" si="11"/>
-        <v>26.51328749999999</v>
+        <v>20.554125000000028</v>
       </c>
       <c r="X40" s="15">
         <f t="shared" si="12"/>
@@ -7790,11 +7799,11 @@
       </c>
       <c r="V41">
         <f t="shared" si="10"/>
-        <v>81.978947500000004</v>
+        <v>82.80182499999998</v>
       </c>
       <c r="W41" s="80">
         <f t="shared" si="11"/>
-        <v>8.0210524999999961</v>
+        <v>7.1981750000000204</v>
       </c>
       <c r="X41" s="15">
         <f t="shared" si="12"/>
@@ -7897,11 +7906,11 @@
       </c>
       <c r="V42">
         <f t="shared" si="10"/>
-        <v>80.865037499999971</v>
+        <v>81.177624999999949</v>
       </c>
       <c r="W42" s="80">
         <f t="shared" si="11"/>
-        <v>-0.86503749999997126</v>
+        <v>-1.1776249999999493</v>
       </c>
       <c r="X42" s="15">
         <f t="shared" si="12"/>
@@ -7928,17 +7937,45 @@
         <v>5.9651476562499965</v>
       </c>
     </row>
+    <row r="43" spans="1:31">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="70"/>
+      <c r="K43" s="72"/>
+      <c r="S43" s="80"/>
+      <c r="U43" s="80"/>
+      <c r="W43" s="80"/>
+    </row>
     <row r="44" spans="1:31">
-      <c r="A44" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44">
-        <f>MIN(C2:C42)</f>
-        <v>10</v>
-      </c>
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="19"/>
+      <c r="S44" s="80"/>
+      <c r="U44" s="80"/>
+      <c r="W44" s="80"/>
     </row>
     <row r="45" spans="1:31">
       <c r="A45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31">
+      <c r="A46" t="s">
         <v>52</v>
       </c>
     </row>
@@ -10005,8 +10042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K56" sqref="A56:K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -14425,8 +14462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15611,8 +15648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:L8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M9" sqref="M6:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17213,7 +17250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M12" sqref="M12"/>
     </sheetView>
@@ -18886,14 +18923,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AD4:AE4"/>
@@ -18904,6 +18933,14 @@
     <mergeCell ref="T4:U4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18916,7 +18953,7 @@
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M24" sqref="B24:M29"/>
+      <selection pane="topRight" activeCell="M24" sqref="A24:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -20647,14 +20684,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="P3:AE3"/>
     <mergeCell ref="AF3:AF5"/>
     <mergeCell ref="P4:Q4"/>
@@ -20665,6 +20694,14 @@
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20675,8 +20712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:M10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M10" sqref="M6:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22279,6 +22316,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="P3:AE3"/>
     <mergeCell ref="AF3:AF5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -22293,10 +22334,6 @@
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:Y4"/>
     <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="P3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23493,8 +23530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M29" sqref="M25:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -25097,6 +25134,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="P3:AE3"/>
     <mergeCell ref="AF3:AF5"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
@@ -25111,10 +25152,6 @@
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:Y4"/>
     <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="P3:AE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hasta conclusiones con los escenarios
</commit_message>
<xml_diff>
--- a/Data-Burgoin.xlsx
+++ b/Data-Burgoin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="11715" windowHeight="7620" firstSheet="4" activeTab="12"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="11715" windowHeight="7620" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="28-04-13" sheetId="1" r:id="rId1"/>
@@ -865,6 +865,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -913,14 +921,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1244,49 +1244,49 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2417,70 +2417,70 @@
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="P3" s="96" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
+      <c r="P3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="87" t="s">
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="91" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2490,42 +2490,42 @@
       <c r="N4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="99" t="s">
+      <c r="P4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="92" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="T4" s="93" t="s">
+      <c r="S4" s="96"/>
+      <c r="T4" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="94"/>
-      <c r="V4" s="92" t="s">
+      <c r="U4" s="98"/>
+      <c r="V4" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="92"/>
-      <c r="X4" s="93" t="s">
+      <c r="W4" s="96"/>
+      <c r="X4" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="92" t="s">
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="93" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="92" t="s">
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="92"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="AE5" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="89"/>
+      <c r="AF5" s="93"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="53">
@@ -3540,49 +3540,49 @@
         <f>SQRT(SUMSQ(O2:O42)/COUNTA(O2:O42))</f>
         <v>29.944844287263219</v>
       </c>
-      <c r="P1" s="100">
+      <c r="P1" s="84">
         <v>4</v>
       </c>
       <c r="Q1" s="79">
         <f>SQRT(SUMSQ(Q2:Q42)/COUNTA(Q2:Q42))</f>
         <v>12.022876428138883</v>
       </c>
-      <c r="R1" s="100">
+      <c r="R1" s="84">
         <v>1</v>
       </c>
       <c r="S1" s="79">
         <f>SQRT(SUMSQ(S2:S42)/COUNTA(S2:S42))</f>
         <v>10.128265491669591</v>
       </c>
-      <c r="T1" s="100">
+      <c r="T1" s="84">
         <v>2</v>
       </c>
       <c r="U1" s="79">
         <f>SQRT(SUMSQ(U2:U42)/COUNTA(U2:U42))</f>
         <v>7.229450832493427</v>
       </c>
-      <c r="V1" s="100">
+      <c r="V1" s="84">
         <v>5</v>
       </c>
       <c r="W1" s="79">
         <f>SQRT(SUMSQ(W2:W42)/COUNTA(W2:W42))</f>
         <v>11.547039077555084</v>
       </c>
-      <c r="X1" s="101">
+      <c r="X1" s="85">
         <v>6</v>
       </c>
-      <c r="Y1" s="102">
+      <c r="Y1" s="86">
         <f>SQRT(SUMSQ(Y2:Y42)/COUNTA(Y2:Y42))</f>
         <v>50.104172608612217</v>
       </c>
-      <c r="Z1" s="101" t="s">
+      <c r="Z1" s="85" t="s">
         <v>53</v>
       </c>
       <c r="AA1" s="79">
         <f>SQRT(SUMSQ(AA2:AA42)/COUNTA(AA2:AA42))</f>
         <v>24.378783529915079</v>
       </c>
-      <c r="AB1" s="100" t="s">
+      <c r="AB1" s="84" t="s">
         <v>54</v>
       </c>
       <c r="AC1" s="79">
@@ -3641,7 +3641,7 @@
         <v>-42.519420000000025</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P44" si="4" xml:space="preserve"> 75 + 0.02937*C2 + 0.017344*E2</f>
+        <f t="shared" ref="P2:P42" si="4" xml:space="preserve"> 75 + 0.02937*C2 + 0.017344*E2</f>
         <v>77.383319999999998</v>
       </c>
       <c r="Q2" s="80">
@@ -3649,7 +3649,7 @@
         <v>-14.383319999999998</v>
       </c>
       <c r="R2">
-        <f t="shared" ref="R2:R44" si="6" xml:space="preserve"> -0.0000003143*(C2)^3 + 0.0005606*(C2)^2 - 0.01602*(C2) + 75.46</f>
+        <f t="shared" ref="R2:R42" si="6" xml:space="preserve"> -0.0000003143*(C2)^3 + 0.0005606*(C2)^2 - 0.01602*(C2) + 75.46</f>
         <v>75.444050886399992</v>
       </c>
       <c r="S2" s="80">
@@ -3657,7 +3657,7 @@
         <v>-12.444050886399992</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T44" si="8" xml:space="preserve"> 76.44 - (0.08533*C2) - (0.003054*E2) + (0.004229*(C2)^2) - (0.002185*C2*E2) + (0.0002715*(E2)^2) - (0.000003174*((C2)^2)*E2) + (0.000001423*C2*(E2)^2) - (0.0000001513*(E2)^3)</f>
+        <f t="shared" ref="T2:T42" si="8" xml:space="preserve"> 76.44 - (0.08533*C2) - (0.003054*E2) + (0.004229*(C2)^2) - (0.002185*C2*E2) + (0.0002715*(E2)^2) - (0.000003174*((C2)^2)*E2) + (0.000001423*C2*(E2)^2) - (0.0000001513*(E2)^3)</f>
         <v>73.77286725999997</v>
       </c>
       <c r="U2" s="80">
@@ -3772,7 +3772,7 @@
         <v>4.802013720000005</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V44" si="10">425 + 0.045635*C3 + 0.01423*E3 - 56.6*A3 + 2.127*G3</f>
+        <f t="shared" ref="V3:V42" si="10">425 + 0.045635*C3 + 0.01423*E3 - 56.6*A3 + 2.127*G3</f>
         <v>76.187254999999993</v>
       </c>
       <c r="W3" s="80">
@@ -3780,7 +3780,7 @@
         <v>1.8127450000000067</v>
       </c>
       <c r="X3" s="15">
-        <f t="shared" ref="X3:X44" si="12" xml:space="preserve"> 95.72 - 1.33*C3 - 0.07005*E3 + 0.04464*C3^2 - 0.01072*C3*E3 + 0.001403*E3^2 - 0.0004819*C3^3 + 0.0002204*C3^2*E3 - 0.00002532*C3*E3^2 + 0.0000009191*C3^4 - 0.0000004632642*C3^3*E3 + 0.00000005263*C3^2*E3^2</f>
+        <f t="shared" ref="X3:X42" si="12" xml:space="preserve"> 95.72 - 1.33*C3 - 0.07005*E3 + 0.04464*C3^2 - 0.01072*C3*E3 + 0.001403*E3^2 - 0.0004819*C3^3 + 0.0002204*C3^2*E3 - 0.00002532*C3*E3^2 + 0.0000009191*C3^4 - 0.0000004632642*C3^3*E3 + 0.00000005263*C3^2*E3^2</f>
         <v>78.570819118692</v>
       </c>
       <c r="Y3" s="15">
@@ -3788,7 +3788,7 @@
         <v>-0.57081911869200042</v>
       </c>
       <c r="Z3" s="15">
-        <f t="shared" ref="Z3:Z44" si="14">(T3+X3)/2</f>
+        <f t="shared" ref="Z3:Z42" si="14">(T3+X3)/2</f>
         <v>75.884402699345998</v>
       </c>
       <c r="AA3" s="80">
@@ -3796,7 +3796,7 @@
         <v>2.1155973006540023</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB44" si="16">(R3+T3)/2</f>
+        <f t="shared" ref="AB3:AB42" si="16">(R3+T3)/2</f>
         <v>74.668429819449997</v>
       </c>
       <c r="AC3" s="80">
@@ -10106,10 +10106,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K56" sqref="A56:K56"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64:K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -14519,8 +14519,957 @@
         <v>9.2095749999999867</v>
       </c>
     </row>
+    <row r="64" spans="1:21">
+      <c r="A64" s="13">
+        <v>7</v>
+      </c>
+      <c r="B64" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="C64" s="15">
+        <v>1500</v>
+      </c>
+      <c r="D64" s="14">
+        <v>5</v>
+      </c>
+      <c r="E64" s="15">
+        <v>9000</v>
+      </c>
+      <c r="F64" s="14">
+        <v>25</v>
+      </c>
+      <c r="G64" s="15">
+        <v>23</v>
+      </c>
+      <c r="H64" s="14">
+        <v>14</v>
+      </c>
+      <c r="I64" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J64" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K64" s="19">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="13">
+        <v>7</v>
+      </c>
+      <c r="B65" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="C65" s="15">
+        <v>570</v>
+      </c>
+      <c r="D65" s="14">
+        <v>4</v>
+      </c>
+      <c r="E65" s="15">
+        <v>3500</v>
+      </c>
+      <c r="F65" s="14">
+        <v>20</v>
+      </c>
+      <c r="G65" s="15">
+        <v>23</v>
+      </c>
+      <c r="H65" s="14">
+        <v>14</v>
+      </c>
+      <c r="I65" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J65" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K65" s="19">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="13">
+        <v>6.9</v>
+      </c>
+      <c r="B66" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="C66" s="15">
+        <v>250</v>
+      </c>
+      <c r="D66" s="14">
+        <v>4</v>
+      </c>
+      <c r="E66" s="15">
+        <v>1800</v>
+      </c>
+      <c r="F66" s="14">
+        <v>20</v>
+      </c>
+      <c r="G66" s="15">
+        <v>22</v>
+      </c>
+      <c r="H66" s="14">
+        <v>14</v>
+      </c>
+      <c r="I66" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J66" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K66" s="19">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="13">
+        <v>7</v>
+      </c>
+      <c r="B67" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="C67" s="15">
+        <v>110</v>
+      </c>
+      <c r="D67" s="14">
+        <v>4</v>
+      </c>
+      <c r="E67" s="15">
+        <v>900</v>
+      </c>
+      <c r="F67" s="14">
+        <v>20</v>
+      </c>
+      <c r="G67" s="15">
+        <v>23</v>
+      </c>
+      <c r="H67" s="14">
+        <v>14</v>
+      </c>
+      <c r="I67" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J67" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K67" s="19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B68" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C68" s="15">
+        <v>400</v>
+      </c>
+      <c r="D68" s="14">
+        <v>3</v>
+      </c>
+      <c r="E68" s="15">
+        <v>700</v>
+      </c>
+      <c r="F68" s="14">
+        <v>15</v>
+      </c>
+      <c r="G68" s="15">
+        <v>27</v>
+      </c>
+      <c r="H68" s="14">
+        <v>22</v>
+      </c>
+      <c r="I68" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J68" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K68" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B69" s="14">
+        <v>6.7</v>
+      </c>
+      <c r="C69" s="15">
+        <v>252</v>
+      </c>
+      <c r="D69" s="14">
+        <v>3</v>
+      </c>
+      <c r="E69" s="15">
+        <v>500</v>
+      </c>
+      <c r="F69" s="14">
+        <v>20</v>
+      </c>
+      <c r="G69" s="15">
+        <v>27</v>
+      </c>
+      <c r="H69" s="14">
+        <v>18</v>
+      </c>
+      <c r="I69" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J69" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K69" s="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B70" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C70" s="15">
+        <v>98</v>
+      </c>
+      <c r="D70" s="14">
+        <v>2</v>
+      </c>
+      <c r="E70" s="15">
+        <v>120</v>
+      </c>
+      <c r="F70" s="14">
+        <v>20</v>
+      </c>
+      <c r="G70" s="15">
+        <v>27</v>
+      </c>
+      <c r="H70" s="14">
+        <v>17</v>
+      </c>
+      <c r="I70" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J70" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K70" s="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B71" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C71" s="15">
+        <v>225</v>
+      </c>
+      <c r="D71" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E71" s="15">
+        <v>300</v>
+      </c>
+      <c r="F71" s="14">
+        <v>30</v>
+      </c>
+      <c r="G71" s="15">
+        <v>27</v>
+      </c>
+      <c r="H71" s="14">
+        <v>23</v>
+      </c>
+      <c r="I71" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J71" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K71" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B72" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C72" s="15">
+        <v>95</v>
+      </c>
+      <c r="D72" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E72" s="15">
+        <v>250</v>
+      </c>
+      <c r="F72" s="14">
+        <v>30</v>
+      </c>
+      <c r="G72" s="15">
+        <v>27</v>
+      </c>
+      <c r="H72" s="14">
+        <v>23</v>
+      </c>
+      <c r="I72" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J72" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K72" s="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="13">
+        <v>6.9</v>
+      </c>
+      <c r="B73" s="14">
+        <v>6.5</v>
+      </c>
+      <c r="C73" s="15">
+        <v>250</v>
+      </c>
+      <c r="D73" s="14">
+        <v>4</v>
+      </c>
+      <c r="E73" s="15">
+        <v>1800</v>
+      </c>
+      <c r="F73" s="14">
+        <v>20</v>
+      </c>
+      <c r="G73" s="15">
+        <v>22</v>
+      </c>
+      <c r="H73" s="14">
+        <v>14</v>
+      </c>
+      <c r="I73" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J73" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K73" s="19">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="13">
+        <v>7</v>
+      </c>
+      <c r="B74" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="C74" s="15">
+        <v>1500</v>
+      </c>
+      <c r="D74" s="14">
+        <v>5</v>
+      </c>
+      <c r="E74" s="15">
+        <v>9000</v>
+      </c>
+      <c r="F74" s="14">
+        <v>25</v>
+      </c>
+      <c r="G74" s="15">
+        <v>23</v>
+      </c>
+      <c r="H74" s="14">
+        <v>14</v>
+      </c>
+      <c r="I74" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J74" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K74" s="19">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="13">
+        <v>7</v>
+      </c>
+      <c r="B75" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="C75" s="15">
+        <v>570</v>
+      </c>
+      <c r="D75" s="14">
+        <v>4</v>
+      </c>
+      <c r="E75" s="15">
+        <v>3500</v>
+      </c>
+      <c r="F75" s="14">
+        <v>20</v>
+      </c>
+      <c r="G75" s="15">
+        <v>23</v>
+      </c>
+      <c r="H75" s="14">
+        <v>14</v>
+      </c>
+      <c r="I75" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J75" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K75" s="19">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="13">
+        <v>7</v>
+      </c>
+      <c r="B76" s="14">
+        <v>6.6</v>
+      </c>
+      <c r="C76" s="15">
+        <v>110</v>
+      </c>
+      <c r="D76" s="14">
+        <v>4</v>
+      </c>
+      <c r="E76" s="15">
+        <v>900</v>
+      </c>
+      <c r="F76" s="14">
+        <v>20</v>
+      </c>
+      <c r="G76" s="15">
+        <v>23</v>
+      </c>
+      <c r="H76" s="14">
+        <v>14</v>
+      </c>
+      <c r="I76" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="J76" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="K76" s="19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B77" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C77" s="15">
+        <v>225</v>
+      </c>
+      <c r="D77" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E77" s="15">
+        <v>300</v>
+      </c>
+      <c r="F77" s="14">
+        <v>30</v>
+      </c>
+      <c r="G77" s="15">
+        <v>27</v>
+      </c>
+      <c r="H77" s="14">
+        <v>23</v>
+      </c>
+      <c r="I77" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J77" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K77" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B78" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C78" s="15">
+        <v>95</v>
+      </c>
+      <c r="D78" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E78" s="15">
+        <v>250</v>
+      </c>
+      <c r="F78" s="14">
+        <v>30</v>
+      </c>
+      <c r="G78" s="15">
+        <v>27</v>
+      </c>
+      <c r="H78" s="14">
+        <v>23</v>
+      </c>
+      <c r="I78" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J78" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K78" s="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B79" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C79" s="15">
+        <v>98</v>
+      </c>
+      <c r="D79" s="14">
+        <v>2</v>
+      </c>
+      <c r="E79" s="15">
+        <v>120</v>
+      </c>
+      <c r="F79" s="14">
+        <v>20</v>
+      </c>
+      <c r="G79" s="15">
+        <v>27</v>
+      </c>
+      <c r="H79" s="14">
+        <v>17</v>
+      </c>
+      <c r="I79" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J79" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K79" s="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B80" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C80" s="15">
+        <v>225</v>
+      </c>
+      <c r="D80" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E80" s="15">
+        <v>300</v>
+      </c>
+      <c r="F80" s="14">
+        <v>30</v>
+      </c>
+      <c r="G80" s="15">
+        <v>27</v>
+      </c>
+      <c r="H80" s="14">
+        <v>23</v>
+      </c>
+      <c r="I80" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J80" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K80" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B81" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C81" s="15">
+        <v>95</v>
+      </c>
+      <c r="D81" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E81" s="15">
+        <v>250</v>
+      </c>
+      <c r="F81" s="14">
+        <v>30</v>
+      </c>
+      <c r="G81" s="15">
+        <v>27</v>
+      </c>
+      <c r="H81" s="14">
+        <v>23</v>
+      </c>
+      <c r="I81" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J81" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K81" s="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B82" s="14">
+        <v>6.7</v>
+      </c>
+      <c r="C82" s="15">
+        <v>252</v>
+      </c>
+      <c r="D82" s="14">
+        <v>3</v>
+      </c>
+      <c r="E82" s="15">
+        <v>500</v>
+      </c>
+      <c r="F82" s="14">
+        <v>20</v>
+      </c>
+      <c r="G82" s="15">
+        <v>27</v>
+      </c>
+      <c r="H82" s="14">
+        <v>18</v>
+      </c>
+      <c r="I82" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J82" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K82" s="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B83" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C83" s="15">
+        <v>400</v>
+      </c>
+      <c r="D83" s="14">
+        <v>3</v>
+      </c>
+      <c r="E83" s="15">
+        <v>700</v>
+      </c>
+      <c r="F83" s="14">
+        <v>15</v>
+      </c>
+      <c r="G83" s="15">
+        <v>27</v>
+      </c>
+      <c r="H83" s="14">
+        <v>22</v>
+      </c>
+      <c r="I83" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J83" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K83" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B84" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C84" s="15">
+        <v>98</v>
+      </c>
+      <c r="D84" s="14">
+        <v>2</v>
+      </c>
+      <c r="E84" s="15">
+        <v>120</v>
+      </c>
+      <c r="F84" s="14">
+        <v>20</v>
+      </c>
+      <c r="G84" s="15">
+        <v>27</v>
+      </c>
+      <c r="H84" s="14">
+        <v>17</v>
+      </c>
+      <c r="I84" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J84" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K84" s="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B85" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C85" s="15">
+        <v>225</v>
+      </c>
+      <c r="D85" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E85" s="15">
+        <v>300</v>
+      </c>
+      <c r="F85" s="14">
+        <v>30</v>
+      </c>
+      <c r="G85" s="15">
+        <v>27</v>
+      </c>
+      <c r="H85" s="14">
+        <v>23</v>
+      </c>
+      <c r="I85" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J85" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K85" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B86" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C86" s="15">
+        <v>95</v>
+      </c>
+      <c r="D86" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E86" s="15">
+        <v>250</v>
+      </c>
+      <c r="F86" s="14">
+        <v>30</v>
+      </c>
+      <c r="G86" s="15">
+        <v>27</v>
+      </c>
+      <c r="H86" s="14">
+        <v>23</v>
+      </c>
+      <c r="I86" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J86" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K86" s="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B87" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C87" s="15">
+        <v>98</v>
+      </c>
+      <c r="D87" s="14">
+        <v>2</v>
+      </c>
+      <c r="E87" s="15">
+        <v>120</v>
+      </c>
+      <c r="F87" s="14">
+        <v>20</v>
+      </c>
+      <c r="G87" s="15">
+        <v>27</v>
+      </c>
+      <c r="H87" s="14">
+        <v>17</v>
+      </c>
+      <c r="I87" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J87" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K87" s="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B88" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C88" s="15">
+        <v>95</v>
+      </c>
+      <c r="D88" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E88" s="15">
+        <v>250</v>
+      </c>
+      <c r="F88" s="14">
+        <v>30</v>
+      </c>
+      <c r="G88" s="15">
+        <v>27</v>
+      </c>
+      <c r="H88" s="14">
+        <v>23</v>
+      </c>
+      <c r="I88" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J88" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K88" s="19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="B89" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C89" s="15">
+        <v>400</v>
+      </c>
+      <c r="D89" s="14">
+        <v>3</v>
+      </c>
+      <c r="E89" s="15">
+        <v>700</v>
+      </c>
+      <c r="F89" s="14">
+        <v>15</v>
+      </c>
+      <c r="G89" s="15">
+        <v>27</v>
+      </c>
+      <c r="H89" s="14">
+        <v>22</v>
+      </c>
+      <c r="I89" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J89" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K89" s="19">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="B90" s="14">
+        <v>6.8</v>
+      </c>
+      <c r="C90" s="15">
+        <v>225</v>
+      </c>
+      <c r="D90" s="14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E90" s="15">
+        <v>300</v>
+      </c>
+      <c r="F90" s="14">
+        <v>30</v>
+      </c>
+      <c r="G90" s="15">
+        <v>27</v>
+      </c>
+      <c r="H90" s="14">
+        <v>23</v>
+      </c>
+      <c r="I90" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J90" s="17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K90" s="19">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A87:K90">
+    <sortCondition ref="K90"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14528,8 +15477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -14549,7 +15498,7 @@
       <c r="A2">
         <v>149.9</v>
       </c>
-      <c r="B2" s="103">
+      <c r="B2" s="87">
         <v>4.2027777777777775</v>
       </c>
       <c r="C2" t="s">
@@ -14569,7 +15518,7 @@
       <c r="A3">
         <v>149.80000000000001</v>
       </c>
-      <c r="B3" s="103">
+      <c r="B3" s="87">
         <v>2.1027777777777779</v>
       </c>
       <c r="C3" t="s">
@@ -14583,7 +15532,7 @@
       <c r="A4">
         <v>149.69999999999999</v>
       </c>
-      <c r="B4" s="103">
+      <c r="B4" s="87">
         <v>1.4020833333333333</v>
       </c>
       <c r="C4" t="s">
@@ -14597,7 +15546,7 @@
       <c r="A5">
         <v>149.6</v>
       </c>
-      <c r="B5" s="103">
+      <c r="B5" s="87">
         <v>1.0527777777777778</v>
       </c>
       <c r="C5" t="s">
@@ -14784,8 +15733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -14800,49 +15749,49 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -14854,7 +15803,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -15968,49 +16917,49 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -16022,7 +16971,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -17524,9 +18473,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F32" sqref="F32"/>
+      <selection pane="topRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17544,70 +18493,70 @@
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="P3" s="96" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
+      <c r="P3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="87" t="s">
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="91" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -17617,42 +18566,42 @@
       <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="99" t="s">
+      <c r="P4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="92" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="T4" s="93" t="s">
+      <c r="S4" s="96"/>
+      <c r="T4" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="94"/>
-      <c r="V4" s="92" t="s">
+      <c r="U4" s="98"/>
+      <c r="V4" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="92"/>
-      <c r="X4" s="93" t="s">
+      <c r="W4" s="96"/>
+      <c r="X4" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="92" t="s">
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="93" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="92" t="s">
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="92"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -17740,7 +18689,7 @@
       <c r="AE5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="89"/>
+      <c r="AF5" s="93"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="12">
@@ -19197,14 +20146,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AD4:AE4"/>
@@ -19215,6 +20156,14 @@
     <mergeCell ref="T4:U4"/>
     <mergeCell ref="V4:W4"/>
     <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19225,9 +20174,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H30" sqref="H30"/>
+      <selection pane="topRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -19242,70 +20191,70 @@
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="P3" s="96" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
+      <c r="P3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="87" t="s">
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="91" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -19315,42 +20264,42 @@
       <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="99" t="s">
+      <c r="P4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="92" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="T4" s="93" t="s">
+      <c r="S4" s="96"/>
+      <c r="T4" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="94"/>
-      <c r="V4" s="92" t="s">
+      <c r="U4" s="98"/>
+      <c r="V4" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="92"/>
-      <c r="X4" s="93" t="s">
+      <c r="W4" s="96"/>
+      <c r="X4" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="92" t="s">
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="93" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="92" t="s">
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="92"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -19438,7 +20387,7 @@
       <c r="AE5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="89"/>
+      <c r="AF5" s="93"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="12">
@@ -20598,40 +21547,40 @@
         <v>7.1</v>
       </c>
       <c r="C24" s="14">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="D24" s="15">
         <v>30</v>
       </c>
       <c r="E24" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F24" s="15">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G24" s="14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H24" s="15">
         <v>27</v>
       </c>
       <c r="I24" s="14">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J24" s="16">
         <v>0.7</v>
       </c>
       <c r="K24" s="17">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="L24" s="18">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="M24" s="19">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="N24" s="17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="P24" s="30"/>
       <c r="Q24" s="31"/>
@@ -20958,14 +21907,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
     <mergeCell ref="P3:AE3"/>
     <mergeCell ref="AF3:AF5"/>
     <mergeCell ref="P4:Q4"/>
@@ -20976,6 +21917,14 @@
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="AB4:AC4"/>
     <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20986,8 +21935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -21002,70 +21951,70 @@
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="P3" s="96" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
+      <c r="P3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="87" t="s">
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="91" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -21075,42 +22024,42 @@
       <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="99" t="s">
+      <c r="P4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="92" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="T4" s="93" t="s">
+      <c r="S4" s="96"/>
+      <c r="T4" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="94"/>
-      <c r="V4" s="92" t="s">
+      <c r="U4" s="98"/>
+      <c r="V4" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="92"/>
-      <c r="X4" s="93" t="s">
+      <c r="W4" s="96"/>
+      <c r="X4" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="92" t="s">
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="93" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="92" t="s">
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="92"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -21198,7 +22147,7 @@
       <c r="AE5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="89"/>
+      <c r="AF5" s="93"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="12">
@@ -22610,6 +23559,7 @@
     <mergeCell ref="V4:W4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22633,49 +23583,49 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -22687,7 +23637,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -23804,8 +24754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M29" sqref="M25:M29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -23820,70 +24770,70 @@
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="85" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="90"/>
+      <c r="L3" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="P3" s="96" t="s">
+      <c r="M3" s="89"/>
+      <c r="N3" s="90"/>
+      <c r="P3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="87" t="s">
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="91" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="84" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91" t="s">
+      <c r="E4" s="94"/>
+      <c r="F4" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="91" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="90"/>
-      <c r="J4" s="85" t="s">
+      <c r="I4" s="94"/>
+      <c r="J4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="86"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
@@ -23893,42 +24843,42 @@
       <c r="N4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="99" t="s">
+      <c r="P4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="92" t="s">
+      <c r="Q4" s="98"/>
+      <c r="R4" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="92"/>
-      <c r="T4" s="93" t="s">
+      <c r="S4" s="96"/>
+      <c r="T4" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="94"/>
-      <c r="V4" s="92" t="s">
+      <c r="U4" s="98"/>
+      <c r="V4" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="92"/>
-      <c r="X4" s="93" t="s">
+      <c r="W4" s="96"/>
+      <c r="X4" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="92" t="s">
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="92"/>
-      <c r="AB4" s="93" t="s">
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="AC4" s="94"/>
-      <c r="AD4" s="92" t="s">
+      <c r="AC4" s="98"/>
+      <c r="AD4" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="88"/>
+      <c r="AE4" s="99"/>
+      <c r="AF4" s="92"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A5" s="89"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -24016,7 +24966,7 @@
       <c r="AE5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="89"/>
+      <c r="AF5" s="93"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="12">

</xml_diff>